<commit_message>
Updated metric variables excel and Bargraphs quarto
</commit_message>
<xml_diff>
--- a/Data/data documentation/Data documentation for council variables.xlsx
+++ b/Data/data documentation/Data documentation for council variables.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10402"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28623"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://drexel0-my.sharepoint.com/personal/tr842_drexel_edu/Documents/Github_repositories/philadelphia-council-districts-and-health/Data/data documentation/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Documents\Github\philadelphia-council-districts-and-health\Data\data documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{E112AF2F-33AB-A34C-AEA7-12F72F04E758}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{590A0218-CF03-4DE1-B1E0-2DAD9B670BD1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2780" yWindow="1500" windowWidth="28040" windowHeight="17440" activeTab="1" xr2:uid="{7E76C4D9-7630-4340-BEBA-4E6127603C3B}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{7E76C4D9-7630-4340-BEBA-4E6127603C3B}"/>
   </bookViews>
   <sheets>
     <sheet name="Data documentation for council " sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="72">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="226" uniqueCount="129">
   <si>
     <t>Map</t>
   </si>
@@ -286,6 +286,224 @@
   </si>
   <si>
     <t xml:space="preserve">Census Block Group aggregated up to the council district using…?... As weights…. </t>
+  </si>
+  <si>
+    <t>Total population</t>
+  </si>
+  <si>
+    <t>Active Business Licenses No Rentals</t>
+  </si>
+  <si>
+    <t>Active Business Licenses Rentals Only</t>
+  </si>
+  <si>
+    <t>Some College</t>
+  </si>
+  <si>
+    <t>College Graduate</t>
+  </si>
+  <si>
+    <t>High School Graduate</t>
+  </si>
+  <si>
+    <t>Less Than High School</t>
+  </si>
+  <si>
+    <t>Code Violations</t>
+  </si>
+  <si>
+    <t>Lack Complete Kitchen</t>
+  </si>
+  <si>
+    <t>Lack Complete Plumbing</t>
+  </si>
+  <si>
+    <t>Median Household Income</t>
+  </si>
+  <si>
+    <t>Owners</t>
+  </si>
+  <si>
+    <t>Renters</t>
+  </si>
+  <si>
+    <t>White</t>
+  </si>
+  <si>
+    <t>Black</t>
+  </si>
+  <si>
+    <t>Native American</t>
+  </si>
+  <si>
+    <t>Asian</t>
+  </si>
+  <si>
+    <t>Pacific Islander</t>
+  </si>
+  <si>
+    <t>Other Race</t>
+  </si>
+  <si>
+    <t>Two or More Races</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Hispanic </t>
+  </si>
+  <si>
+    <t>Fatal Shootings</t>
+  </si>
+  <si>
+    <t>Nonfatal Shootings</t>
+  </si>
+  <si>
+    <t>Uninsured</t>
+  </si>
+  <si>
+    <t>Tree Canopy Coverage</t>
+  </si>
+  <si>
+    <t>Heat Vulnerabillity Index</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Variables Used: 
+#"B15003_001" = total pop over 25
+#"B15003_002" = No schooling
+#"B15003_003" = Nursery School 
+#"B15003_004"= Kindergarten
+#"B15003_005" = 1st
+#"B15003_006" = 2nd, 
+#"B15003_007" = 3rd 
+#"B15003_008" = 4th, 
+#"B15003_009" = 5th, 
+#"B15003_010" = 6th
+#"B15003_011" = 7th 
+#"B15003_012"= 8th 
+#"B15003_013" 9th 
+#"B15003_014"= 10th 
+#"B15003_015" = 11th
+#"B15003_016" = 12th no diploma 
+</t>
+  </si>
+  <si>
+    <t>Total Population over the Age of 25</t>
+  </si>
+  <si>
+    <t>Percentage of residents over the age of 25 with less than High school for highest educational attainment</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Variables Used:
+#"B15003_001" = total pop over 25,
+#"B15003_017" HS grad, 
+#"B15003_018" = GED or equivalent </t>
+  </si>
+  <si>
+    <t>Percentage of residents over the age of 25 with High school Diploma or equivalent for highest educational attainment</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Variables Used:
+#"B15003_001" = total pop over 25,
+#"B15003_019" = some college less than 1 yr
+#"B15003_020"= some college 1 yr or more no degree
+#"B15003_021"= Associates </t>
+  </si>
+  <si>
+    <t>Percentage of residents over the age of 25 with some college for highest educational attainment</t>
+  </si>
+  <si>
+    <t>Percentage of residents over the age of 25 with a bachelor's degree or higher for highest educational attainment</t>
+  </si>
+  <si>
+    <t>Variables Used: 
+#"B15003_001" = total pop over 25,
+#"B15003_022"= Bachelors 
+#"B15003_023"= Masters 
+#"B15003_024"= Professional school 
+#"B15003_025" = Doctorate</t>
+  </si>
+  <si>
+    <t>Census Block Group aggregated up to the council district using Block population as weights</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Total Population  </t>
+  </si>
+  <si>
+    <t>Variables Used:
+#B02001_001 Total pop
+#B03002_003 White Not hispanic or Latino</t>
+  </si>
+  <si>
+    <t>Variables Used:
+#B02001_001 Total pop,
+#B02001_003 Black</t>
+  </si>
+  <si>
+    <t>Variables Used:
+#B02001_001 Total pop,
+#B02001_004 American Indian/Alaska Native</t>
+  </si>
+  <si>
+    <t>Variables Used:
+#B02001_001 Total pop,
+#B02001_005 Asian</t>
+  </si>
+  <si>
+    <t>Variables Used:
+#B02001_001 Total pop,
+#B02001_006 Native Hawaiian/Pacific Islander</t>
+  </si>
+  <si>
+    <t>Variables Used:
+#B02001_001 Total pop,
+#B02001_007 Some other race</t>
+  </si>
+  <si>
+    <t>Variables Used:
+#B02001_001 Total pop,
+#B02001_008 Two or more races</t>
+  </si>
+  <si>
+    <t>Variables Used:
+#B03001_001 Total pop,
+#B03002_012 Hispanic/Latino</t>
+  </si>
+  <si>
+    <t>Percentage of residents who are Native Indian/Alaska Native, non-hispanic</t>
+  </si>
+  <si>
+    <t>Percentage of residents who are Black, Non-hispanic</t>
+  </si>
+  <si>
+    <t>Percentage of residents who are White, Non-hispanic</t>
+  </si>
+  <si>
+    <t>Percentage of residents who are Asian, Non-hispanic</t>
+  </si>
+  <si>
+    <t>Percentage of residents who are Pacific Islander/Native Hawaiian, Non-hispanic</t>
+  </si>
+  <si>
+    <t>Percentage of residents who are other race, Non-hispanic</t>
+  </si>
+  <si>
+    <t>Percentage of residents who are two or more races, Non-hispanic</t>
+  </si>
+  <si>
+    <t>Percentage of residents who are Hispanic</t>
+  </si>
+  <si>
+    <t>Variables Used:
+#B17001_002 #Estimate!!Total:!!Income in the past 12 months below poverty level:
+#B17001_001 #Estimate: Total</t>
+  </si>
+  <si>
+    <t>Percentage of Residents who are below the poverty level</t>
+  </si>
+  <si>
+    <t>Total Population</t>
+  </si>
+  <si>
+    <t>Census Tract aggregated up to the council district using Block population as weights</t>
   </si>
 </sst>
 </file>
@@ -789,7 +1007,7 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -808,6 +1026,9 @@
     <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1185,22 +1406,22 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{01CB8890-B7A9-3A40-979C-A48DC9A37105}">
   <dimension ref="A1:H27"/>
   <sheetViews>
-    <sheetView topLeftCell="A5" workbookViewId="0">
+    <sheetView topLeftCell="A3" workbookViewId="0">
       <selection activeCell="A23" sqref="A23:G29"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="24.5" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="20.1640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="21.83203125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="13.83203125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="11.33203125" customWidth="1"/>
-    <col min="6" max="6" width="27.1640625" customWidth="1"/>
-    <col min="7" max="7" width="15.1640625" customWidth="1"/>
+    <col min="2" max="2" width="20.19921875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="21.796875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.796875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.296875" customWidth="1"/>
+    <col min="6" max="6" width="27.19921875" customWidth="1"/>
+    <col min="7" max="7" width="15.19921875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1223,7 +1444,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>7</v>
       </c>
@@ -1246,7 +1467,7 @@
         <v>45716</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:7" ht="265.2" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>12</v>
       </c>
@@ -1269,7 +1490,7 @@
         <v>45725</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:7" ht="358.8" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>17</v>
       </c>
@@ -1292,7 +1513,7 @@
         <v>45726</v>
       </c>
     </row>
-    <row r="5" spans="1:7" ht="102" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:7" ht="187.2" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>20</v>
       </c>
@@ -1315,7 +1536,7 @@
         <v>45718</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:7" ht="409.6" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>23</v>
       </c>
@@ -1338,7 +1559,7 @@
         <v>45719</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:7" ht="409.6" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>27</v>
       </c>
@@ -1361,7 +1582,7 @@
         <v>45719</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>30</v>
       </c>
@@ -1384,7 +1605,7 @@
         <v>45719</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>35</v>
       </c>
@@ -1404,7 +1625,7 @@
         <v>45719</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:7" ht="409.6" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>38</v>
       </c>
@@ -1427,7 +1648,7 @@
         <v>45725</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>41</v>
       </c>
@@ -1450,7 +1671,7 @@
         <v>45725</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>46</v>
       </c>
@@ -1473,7 +1694,7 @@
         <v>45726</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>50</v>
       </c>
@@ -1496,7 +1717,7 @@
         <v>45725</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:7" ht="296.39999999999998" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>54</v>
       </c>
@@ -1519,7 +1740,7 @@
         <v>45726</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:7" ht="187.2" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>57</v>
       </c>
@@ -1542,7 +1763,7 @@
         <v>45726</v>
       </c>
     </row>
-    <row r="26" spans="1:8" s="5" customFormat="1" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:8" s="5" customFormat="1" ht="19.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A26" s="4"/>
       <c r="B26" s="4"/>
       <c r="C26" s="4"/>
@@ -1552,7 +1773,7 @@
       <c r="G26" s="4"/>
       <c r="H26" s="4"/>
     </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A27" s="3"/>
       <c r="B27" s="3"/>
       <c r="C27" s="3"/>
@@ -1569,21 +1790,23 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B07AACCA-88DB-7C45-AECA-8998520502A5}">
-  <dimension ref="A1:G2"/>
+  <dimension ref="A1:G30"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G5" sqref="G5"/>
+      <selection activeCell="G28" sqref="G28"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="20.33203125" customWidth="1"/>
-    <col min="3" max="3" width="22.33203125" customWidth="1"/>
-    <col min="6" max="6" width="19.6640625" customWidth="1"/>
-    <col min="7" max="7" width="16" customWidth="1"/>
+    <col min="1" max="1" width="20.19921875" style="2" customWidth="1"/>
+    <col min="2" max="2" width="20.296875" style="2" customWidth="1"/>
+    <col min="3" max="3" width="22.296875" style="2" customWidth="1"/>
+    <col min="4" max="5" width="11.19921875" style="2"/>
+    <col min="6" max="6" width="19.69921875" customWidth="1"/>
+    <col min="7" max="7" width="30" style="10" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="68" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:7" ht="46.8" x14ac:dyDescent="0.3">
       <c r="A1" s="6" t="s">
         <v>60</v>
       </c>
@@ -1602,11 +1825,11 @@
       <c r="F1" s="6" t="s">
         <v>70</v>
       </c>
-      <c r="G1" s="6" t="s">
+      <c r="G1" s="8" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:7" ht="85" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:7" ht="78" x14ac:dyDescent="0.3">
       <c r="A2" s="7" t="s">
         <v>20</v>
       </c>
@@ -1625,8 +1848,466 @@
       <c r="F2" s="7" t="s">
         <v>71</v>
       </c>
-      <c r="G2" s="7" t="s">
+      <c r="G2" s="9" t="s">
         <v>68</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A3" s="2" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" ht="31.2" x14ac:dyDescent="0.3">
+      <c r="A4" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="E4" s="2" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" ht="31.2" x14ac:dyDescent="0.3">
+      <c r="A5" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="E5" s="2" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" ht="31.2" x14ac:dyDescent="0.3">
+      <c r="A6" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="D6" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="E6" s="2" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" ht="280.8" x14ac:dyDescent="0.3">
+      <c r="A7" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>99</v>
+      </c>
+      <c r="D7" s="7" t="s">
+        <v>67</v>
+      </c>
+      <c r="E7" s="7" t="s">
+        <v>66</v>
+      </c>
+      <c r="F7" s="2" t="s">
+        <v>107</v>
+      </c>
+      <c r="G7" s="2" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" ht="78" x14ac:dyDescent="0.3">
+      <c r="A8" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>102</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>99</v>
+      </c>
+      <c r="D8" s="7" t="s">
+        <v>67</v>
+      </c>
+      <c r="E8" s="7" t="s">
+        <v>66</v>
+      </c>
+      <c r="F8" s="2" t="s">
+        <v>107</v>
+      </c>
+      <c r="G8" s="2" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" ht="109.2" x14ac:dyDescent="0.3">
+      <c r="A9" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>104</v>
+      </c>
+      <c r="C9" s="2" t="s">
+        <v>99</v>
+      </c>
+      <c r="D9" s="7" t="s">
+        <v>67</v>
+      </c>
+      <c r="E9" s="7" t="s">
+        <v>66</v>
+      </c>
+      <c r="F9" s="2" t="s">
+        <v>107</v>
+      </c>
+      <c r="G9" s="2" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" ht="109.2" x14ac:dyDescent="0.3">
+      <c r="A10" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="C10" s="2" t="s">
+        <v>99</v>
+      </c>
+      <c r="D10" s="7" t="s">
+        <v>67</v>
+      </c>
+      <c r="E10" s="7" t="s">
+        <v>66</v>
+      </c>
+      <c r="F10" s="2" t="s">
+        <v>107</v>
+      </c>
+      <c r="G10" s="2" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" ht="31.2" x14ac:dyDescent="0.3">
+      <c r="A11" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="D11" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="E11" s="7" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A12" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="D12" s="7" t="s">
+        <v>67</v>
+      </c>
+      <c r="E12" s="7" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" ht="31.2" x14ac:dyDescent="0.3">
+      <c r="A13" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="D13" s="7" t="s">
+        <v>67</v>
+      </c>
+      <c r="E13" s="7" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" ht="31.2" x14ac:dyDescent="0.3">
+      <c r="A14" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="D14" s="7" t="s">
+        <v>67</v>
+      </c>
+      <c r="E14" s="7" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A15" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="D15" s="7" t="s">
+        <v>67</v>
+      </c>
+      <c r="E15" s="7" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A16" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="D16" s="7" t="s">
+        <v>67</v>
+      </c>
+      <c r="E16" s="7" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" ht="78" x14ac:dyDescent="0.3">
+      <c r="A17" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="B17" s="2" t="s">
+        <v>119</v>
+      </c>
+      <c r="C17" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="D17" s="7" t="s">
+        <v>67</v>
+      </c>
+      <c r="E17" s="7" t="s">
+        <v>66</v>
+      </c>
+      <c r="F17" s="2" t="s">
+        <v>107</v>
+      </c>
+      <c r="G17" s="2" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" ht="78" x14ac:dyDescent="0.3">
+      <c r="A18" s="2" t="s">
+        <v>86</v>
+      </c>
+      <c r="B18" s="2" t="s">
+        <v>118</v>
+      </c>
+      <c r="C18" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="D18" s="7" t="s">
+        <v>67</v>
+      </c>
+      <c r="E18" s="7" t="s">
+        <v>66</v>
+      </c>
+      <c r="F18" s="2" t="s">
+        <v>107</v>
+      </c>
+      <c r="G18" s="2" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" ht="78" x14ac:dyDescent="0.3">
+      <c r="A19" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="B19" s="2" t="s">
+        <v>117</v>
+      </c>
+      <c r="C19" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="D19" s="7" t="s">
+        <v>67</v>
+      </c>
+      <c r="E19" s="7" t="s">
+        <v>66</v>
+      </c>
+      <c r="F19" s="2" t="s">
+        <v>107</v>
+      </c>
+      <c r="G19" s="2" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" ht="78" x14ac:dyDescent="0.3">
+      <c r="A20" s="2" t="s">
+        <v>88</v>
+      </c>
+      <c r="B20" s="2" t="s">
+        <v>120</v>
+      </c>
+      <c r="C20" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="D20" s="7" t="s">
+        <v>67</v>
+      </c>
+      <c r="E20" s="7" t="s">
+        <v>66</v>
+      </c>
+      <c r="F20" s="2" t="s">
+        <v>107</v>
+      </c>
+      <c r="G20" s="2" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" ht="78" x14ac:dyDescent="0.3">
+      <c r="A21" s="2" t="s">
+        <v>89</v>
+      </c>
+      <c r="B21" s="2" t="s">
+        <v>121</v>
+      </c>
+      <c r="C21" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="D21" s="7" t="s">
+        <v>67</v>
+      </c>
+      <c r="E21" s="7" t="s">
+        <v>66</v>
+      </c>
+      <c r="F21" s="2" t="s">
+        <v>107</v>
+      </c>
+      <c r="G21" s="2" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" ht="78" x14ac:dyDescent="0.3">
+      <c r="A22" s="2" t="s">
+        <v>90</v>
+      </c>
+      <c r="B22" s="2" t="s">
+        <v>122</v>
+      </c>
+      <c r="C22" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="D22" s="7" t="s">
+        <v>67</v>
+      </c>
+      <c r="E22" s="7" t="s">
+        <v>66</v>
+      </c>
+      <c r="F22" s="2" t="s">
+        <v>107</v>
+      </c>
+      <c r="G22" s="2" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" ht="78" x14ac:dyDescent="0.3">
+      <c r="A23" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="B23" s="2" t="s">
+        <v>123</v>
+      </c>
+      <c r="C23" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="D23" s="7" t="s">
+        <v>67</v>
+      </c>
+      <c r="E23" s="7" t="s">
+        <v>66</v>
+      </c>
+      <c r="F23" s="2" t="s">
+        <v>107</v>
+      </c>
+      <c r="G23" s="2" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" ht="78" x14ac:dyDescent="0.3">
+      <c r="A24" s="2" t="s">
+        <v>92</v>
+      </c>
+      <c r="B24" s="2" t="s">
+        <v>124</v>
+      </c>
+      <c r="C24" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="D24" s="7" t="s">
+        <v>67</v>
+      </c>
+      <c r="E24" s="7" t="s">
+        <v>66</v>
+      </c>
+      <c r="F24" s="2" t="s">
+        <v>107</v>
+      </c>
+      <c r="G24" s="2" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" ht="31.2" x14ac:dyDescent="0.3">
+      <c r="A25" s="2" t="s">
+        <v>93</v>
+      </c>
+      <c r="D25" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="E25" s="7" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" ht="31.2" x14ac:dyDescent="0.3">
+      <c r="A26" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="D26" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="E26" s="7" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A27" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="D27" s="7" t="s">
+        <v>67</v>
+      </c>
+      <c r="E27" s="7" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A28" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="D28" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="E28" s="2">
+        <v>2019</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" ht="31.2" x14ac:dyDescent="0.3">
+      <c r="A29" s="2" t="s">
+        <v>97</v>
+      </c>
+      <c r="D29" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="E29" s="2">
+        <v>2018</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7" ht="78" x14ac:dyDescent="0.3">
+      <c r="A30" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="B30" s="2" t="s">
+        <v>126</v>
+      </c>
+      <c r="C30" s="2" t="s">
+        <v>127</v>
+      </c>
+      <c r="D30" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="E30" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="F30" s="2" t="s">
+        <v>128</v>
+      </c>
+      <c r="G30" s="2" t="s">
+        <v>125</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updated/Finished Data Documentation for Variables
</commit_message>
<xml_diff>
--- a/Data/data documentation/Data documentation for council variables.xlsx
+++ b/Data/data documentation/Data documentation for council variables.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Documents\Github\philadelphia-council-districts-and-health\Data\data documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{590A0218-CF03-4DE1-B1E0-2DAD9B670BD1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AD9CA299-A8C7-41BE-AB11-32068B0DBC82}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{7E76C4D9-7630-4340-BEBA-4E6127603C3B}"/>
   </bookViews>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="226" uniqueCount="129">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="276" uniqueCount="158">
   <si>
     <t>Map</t>
   </si>
@@ -504,6 +504,109 @@
   </si>
   <si>
     <t>Census Tract aggregated up to the council district using Block population as weights</t>
+  </si>
+  <si>
+    <t>Count of Licenses</t>
+  </si>
+  <si>
+    <t>Counts already at the council district level</t>
+  </si>
+  <si>
+    <t>Count of crashes</t>
+  </si>
+  <si>
+    <t>Counts were summarized per council district using a spatial join</t>
+  </si>
+  <si>
+    <t>Percentage of buildings with an open housing code violation</t>
+  </si>
+  <si>
+    <t>The number of parcels of land available per council district</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Code violations were set at the council district level. However land parcels had to be spatially joined to council districts. </t>
+  </si>
+  <si>
+    <t>Percentage of homes that lack a complete kitchen</t>
+  </si>
+  <si>
+    <t>Percentage of homes that lack complete plumbing</t>
+  </si>
+  <si>
+    <t>Census Block Group aggregated up to the council district using total number of households as weights</t>
+  </si>
+  <si>
+    <t>Variables Used:
+#B25048_001 --&gt; Total Occupied housing units tract
+#B25048_003 --&gt; Lacking plumbing occupied housing units tract</t>
+  </si>
+  <si>
+    <t>Variables Used:
+#B25052_001 --&gt; Total Occupied housing units tract
+#B25052_003 --&gt; Lacking complete kitchen facilities tract</t>
+  </si>
+  <si>
+    <t>Total Number of Occupied Housing Units</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Variables Used:
+#B19013_001 - Estimate!!Median household income in the past 12 months (in 2022 inflation-adjusted dollars)
+</t>
+  </si>
+  <si>
+    <t>Variables Used:
+#B25003_001 --&gt; Estimate!!Total: block group
+#B25003_002 --&gt; Estimate!!Total:!!Owner occupied block group</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Variables Used:
+#B25003_001 --&gt; Estimate!!Total: block group
+#B25003_003 --&gt; Estimate!!Total:!!Renter occupied block group </t>
+  </si>
+  <si>
+    <t>Total Number of Households</t>
+  </si>
+  <si>
+    <t>Percentage of Households that Own their home</t>
+  </si>
+  <si>
+    <t>Percentage of Households that Rent their home</t>
+  </si>
+  <si>
+    <t>Total Number of Fatal Shootings per Council District</t>
+  </si>
+  <si>
+    <t>Total Number of Nonfatal Shootings per Council District</t>
+  </si>
+  <si>
+    <t>Variables Used:
+#B18135_007 -- Estimate!!Total:!!Under 19 years:!!With a disability:!!No health insurance coverage
+#B18135_012 -- Estimate!!Total:!!Under 19 years:!!No disability:!!No health insurance coverage
+#B18135_018 -- Estimate!!Total:!!19 to 64 years:!!With a disability:!!No health insurance coverage
+#B18135_023 -- Estimate!!Total:!!19 to 64 years:!!No disability:!!No health insurance coverage
+#B18135_029 -- Estimate!!Total:!!65 years and over:!!With a disability:!!No health insurance coverage
+#B18135_034 -- Estimate!!Total:!!65 years and over:!!No disability:!!No health insurance coverage</t>
+  </si>
+  <si>
+    <t>Block Group variables were aggregated up to the council district level using Block population as the weights</t>
+  </si>
+  <si>
+    <t>Total Number of People</t>
+  </si>
+  <si>
+    <t>Percentage of people Uninsured</t>
+  </si>
+  <si>
+    <t>Used IPUMS crosswalk to convert 2010 Census tracts to 2020 Blocks. Before joining at the council district level</t>
+  </si>
+  <si>
+    <t>Percentage of Council district covered by greenspace</t>
+  </si>
+  <si>
+    <t>Shape Area of Council District</t>
+  </si>
+  <si>
+    <t>2010 Census tracts, converted to 2020 Blocks, then aggregated up to the council district level using 2010 Shape Area as weights</t>
   </si>
 </sst>
 </file>
@@ -1007,7 +1110,7 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -1026,9 +1129,8 @@
     <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1793,7 +1895,7 @@
   <dimension ref="A1:G30"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G28" sqref="G28"/>
+      <selection activeCell="G30" sqref="G30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -1803,7 +1905,7 @@
     <col min="3" max="3" width="22.296875" style="2" customWidth="1"/>
     <col min="4" max="5" width="11.19921875" style="2"/>
     <col min="6" max="6" width="19.69921875" customWidth="1"/>
-    <col min="7" max="7" width="30" style="10" customWidth="1"/>
+    <col min="7" max="7" width="30" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="46.8" x14ac:dyDescent="0.3">
@@ -1861,33 +1963,60 @@
       <c r="A4" s="2" t="s">
         <v>73</v>
       </c>
+      <c r="B4" s="2" t="s">
+        <v>129</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>65</v>
+      </c>
       <c r="D4" s="2" t="s">
         <v>8</v>
       </c>
       <c r="E4" s="2" t="s">
         <v>43</v>
+      </c>
+      <c r="F4" s="2" t="s">
+        <v>130</v>
       </c>
     </row>
     <row r="5" spans="1:7" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A5" s="2" t="s">
         <v>74</v>
       </c>
+      <c r="B5" s="2" t="s">
+        <v>129</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>65</v>
+      </c>
       <c r="D5" s="2" t="s">
         <v>8</v>
       </c>
       <c r="E5" s="2" t="s">
         <v>43</v>
       </c>
-    </row>
-    <row r="6" spans="1:7" ht="31.2" x14ac:dyDescent="0.3">
+      <c r="F5" s="2" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" ht="62.4" x14ac:dyDescent="0.3">
       <c r="A6" s="2" t="s">
         <v>30</v>
       </c>
+      <c r="B6" s="2" t="s">
+        <v>131</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>65</v>
+      </c>
       <c r="D6" s="2" t="s">
         <v>8</v>
       </c>
       <c r="E6" s="2" t="s">
         <v>32</v>
+      </c>
+      <c r="F6" s="2" t="s">
+        <v>132</v>
       </c>
     </row>
     <row r="7" spans="1:7" ht="280.8" x14ac:dyDescent="0.3">
@@ -1982,70 +2111,139 @@
         <v>106</v>
       </c>
     </row>
-    <row r="11" spans="1:7" ht="31.2" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:7" ht="93.6" x14ac:dyDescent="0.3">
       <c r="A11" s="2" t="s">
         <v>79</v>
       </c>
+      <c r="B11" s="2" t="s">
+        <v>133</v>
+      </c>
+      <c r="C11" s="2" t="s">
+        <v>134</v>
+      </c>
       <c r="D11" s="2" t="s">
         <v>8</v>
       </c>
       <c r="E11" s="7" t="s">
         <v>51</v>
       </c>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="F11" s="2" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" ht="78" x14ac:dyDescent="0.3">
       <c r="A12" s="2" t="s">
         <v>80</v>
       </c>
+      <c r="B12" s="2" t="s">
+        <v>136</v>
+      </c>
+      <c r="C12" s="2" t="s">
+        <v>141</v>
+      </c>
       <c r="D12" s="7" t="s">
         <v>67</v>
       </c>
       <c r="E12" s="7" t="s">
         <v>66</v>
       </c>
-    </row>
-    <row r="13" spans="1:7" ht="31.2" x14ac:dyDescent="0.3">
+      <c r="F12" s="2" t="s">
+        <v>128</v>
+      </c>
+      <c r="G12" s="2" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" ht="78" x14ac:dyDescent="0.3">
       <c r="A13" s="2" t="s">
         <v>81</v>
       </c>
+      <c r="B13" s="2" t="s">
+        <v>137</v>
+      </c>
+      <c r="C13" s="2" t="s">
+        <v>141</v>
+      </c>
       <c r="D13" s="7" t="s">
         <v>67</v>
       </c>
       <c r="E13" s="7" t="s">
         <v>66</v>
       </c>
-    </row>
-    <row r="14" spans="1:7" ht="31.2" x14ac:dyDescent="0.3">
+      <c r="F13" s="2" t="s">
+        <v>128</v>
+      </c>
+      <c r="G13" s="2" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" ht="93.6" x14ac:dyDescent="0.3">
       <c r="A14" s="2" t="s">
         <v>82</v>
       </c>
+      <c r="B14" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="C14" s="2" t="s">
+        <v>65</v>
+      </c>
       <c r="D14" s="7" t="s">
         <v>67</v>
       </c>
       <c r="E14" s="7" t="s">
         <v>66</v>
       </c>
-    </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="F14" s="2" t="s">
+        <v>138</v>
+      </c>
+      <c r="G14" s="2" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" ht="93.6" x14ac:dyDescent="0.3">
       <c r="A15" s="2" t="s">
         <v>83</v>
       </c>
+      <c r="B15" s="2" t="s">
+        <v>146</v>
+      </c>
+      <c r="C15" s="2" t="s">
+        <v>145</v>
+      </c>
       <c r="D15" s="7" t="s">
         <v>67</v>
       </c>
       <c r="E15" s="7" t="s">
         <v>66</v>
       </c>
-    </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="F15" s="2" t="s">
+        <v>138</v>
+      </c>
+      <c r="G15" s="2" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" ht="93.6" x14ac:dyDescent="0.3">
       <c r="A16" s="2" t="s">
         <v>84</v>
       </c>
+      <c r="B16" s="2" t="s">
+        <v>147</v>
+      </c>
+      <c r="C16" s="2" t="s">
+        <v>145</v>
+      </c>
       <c r="D16" s="7" t="s">
         <v>67</v>
       </c>
       <c r="E16" s="7" t="s">
         <v>66</v>
+      </c>
+      <c r="F16" s="2" t="s">
+        <v>138</v>
+      </c>
+      <c r="G16" s="2" t="s">
+        <v>144</v>
       </c>
     </row>
     <row r="17" spans="1:7" ht="78" x14ac:dyDescent="0.3">
@@ -2232,59 +2430,113 @@
         <v>116</v>
       </c>
     </row>
-    <row r="25" spans="1:7" ht="31.2" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:7" ht="62.4" x14ac:dyDescent="0.3">
       <c r="A25" s="2" t="s">
         <v>93</v>
       </c>
+      <c r="B25" s="2" t="s">
+        <v>148</v>
+      </c>
+      <c r="C25" s="2" t="s">
+        <v>65</v>
+      </c>
       <c r="D25" s="2" t="s">
         <v>8</v>
       </c>
       <c r="E25" s="7" t="s">
         <v>47</v>
       </c>
-    </row>
-    <row r="26" spans="1:7" ht="31.2" x14ac:dyDescent="0.3">
+      <c r="F25" s="2" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" ht="62.4" x14ac:dyDescent="0.3">
       <c r="A26" s="2" t="s">
         <v>94</v>
       </c>
+      <c r="B26" s="2" t="s">
+        <v>149</v>
+      </c>
+      <c r="C26" s="2" t="s">
+        <v>65</v>
+      </c>
       <c r="D26" s="2" t="s">
         <v>8</v>
       </c>
       <c r="E26" s="7" t="s">
         <v>47</v>
       </c>
-    </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="F26" s="2" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" ht="409.6" x14ac:dyDescent="0.3">
       <c r="A27" s="2" t="s">
         <v>95</v>
       </c>
+      <c r="B27" s="2" t="s">
+        <v>153</v>
+      </c>
+      <c r="C27" s="2" t="s">
+        <v>152</v>
+      </c>
       <c r="D27" s="7" t="s">
         <v>67</v>
       </c>
       <c r="E27" s="7" t="s">
         <v>66</v>
       </c>
-    </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="F27" s="2" t="s">
+        <v>151</v>
+      </c>
+      <c r="G27" s="2" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" ht="109.2" x14ac:dyDescent="0.3">
       <c r="A28" s="2" t="s">
         <v>96</v>
       </c>
+      <c r="B28" s="2" t="s">
+        <v>155</v>
+      </c>
+      <c r="C28" s="2" t="s">
+        <v>156</v>
+      </c>
       <c r="D28" s="2" t="s">
         <v>36</v>
       </c>
       <c r="E28" s="2">
         <v>2019</v>
       </c>
-    </row>
-    <row r="29" spans="1:7" ht="31.2" x14ac:dyDescent="0.3">
+      <c r="F28" s="2" t="s">
+        <v>157</v>
+      </c>
+      <c r="G28" s="2" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" ht="109.2" x14ac:dyDescent="0.3">
       <c r="A29" s="2" t="s">
         <v>97</v>
       </c>
+      <c r="B29" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C29" s="2" t="s">
+        <v>65</v>
+      </c>
       <c r="D29" s="2" t="s">
         <v>8</v>
       </c>
       <c r="E29" s="2">
         <v>2018</v>
+      </c>
+      <c r="F29" s="2" t="s">
+        <v>157</v>
+      </c>
+      <c r="G29" s="2" t="s">
+        <v>154</v>
       </c>
     </row>
     <row r="30" spans="1:7" ht="78" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
Updated data documentation for Race Variables to reflect PRD
</commit_message>
<xml_diff>
--- a/Data/data documentation/Data documentation for council variables.xlsx
+++ b/Data/data documentation/Data documentation for council variables.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28623"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28730"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Documents\Github\philadelphia-council-districts-and-health\Data\data documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AD9CA299-A8C7-41BE-AB11-32068B0DBC82}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{925B5796-3466-4522-AE1C-06CF5B143E71}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{7E76C4D9-7630-4340-BEBA-4E6127603C3B}"/>
   </bookViews>
@@ -468,25 +468,7 @@
 #B03002_012 Hispanic/Latino</t>
   </si>
   <si>
-    <t>Percentage of residents who are Native Indian/Alaska Native, non-hispanic</t>
-  </si>
-  <si>
-    <t>Percentage of residents who are Black, Non-hispanic</t>
-  </si>
-  <si>
     <t>Percentage of residents who are White, Non-hispanic</t>
-  </si>
-  <si>
-    <t>Percentage of residents who are Asian, Non-hispanic</t>
-  </si>
-  <si>
-    <t>Percentage of residents who are Pacific Islander/Native Hawaiian, Non-hispanic</t>
-  </si>
-  <si>
-    <t>Percentage of residents who are other race, Non-hispanic</t>
-  </si>
-  <si>
-    <t>Percentage of residents who are two or more races, Non-hispanic</t>
   </si>
   <si>
     <t>Percentage of residents who are Hispanic</t>
@@ -607,6 +589,24 @@
   </si>
   <si>
     <t>2010 Census tracts, converted to 2020 Blocks, then aggregated up to the council district level using 2010 Shape Area as weights</t>
+  </si>
+  <si>
+    <t>Percentage of residents who are Black</t>
+  </si>
+  <si>
+    <t>Percentage of residents who are Native Indian/Alaska Native</t>
+  </si>
+  <si>
+    <t>Percentage of residents who are Asian</t>
+  </si>
+  <si>
+    <t>Percentage of residents who are Pacific Islander/Native Hawaiian</t>
+  </si>
+  <si>
+    <t>Percentage of residents who are other race</t>
+  </si>
+  <si>
+    <t>Percentage of residents who are two or more races</t>
   </si>
 </sst>
 </file>
@@ -1894,8 +1894,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B07AACCA-88DB-7C45-AECA-8998520502A5}">
   <dimension ref="A1:G30"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G30" sqref="G30"/>
+    <sheetView tabSelected="1" topLeftCell="A20" workbookViewId="0">
+      <selection activeCell="B23" sqref="B23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -1964,7 +1964,7 @@
         <v>73</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>129</v>
+        <v>123</v>
       </c>
       <c r="C4" s="2" t="s">
         <v>65</v>
@@ -1976,7 +1976,7 @@
         <v>43</v>
       </c>
       <c r="F4" s="2" t="s">
-        <v>130</v>
+        <v>124</v>
       </c>
     </row>
     <row r="5" spans="1:7" ht="31.2" x14ac:dyDescent="0.3">
@@ -1984,7 +1984,7 @@
         <v>74</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>129</v>
+        <v>123</v>
       </c>
       <c r="C5" s="2" t="s">
         <v>65</v>
@@ -1996,7 +1996,7 @@
         <v>43</v>
       </c>
       <c r="F5" s="2" t="s">
-        <v>130</v>
+        <v>124</v>
       </c>
     </row>
     <row r="6" spans="1:7" ht="62.4" x14ac:dyDescent="0.3">
@@ -2004,7 +2004,7 @@
         <v>30</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>131</v>
+        <v>125</v>
       </c>
       <c r="C6" s="2" t="s">
         <v>65</v>
@@ -2016,7 +2016,7 @@
         <v>32</v>
       </c>
       <c r="F6" s="2" t="s">
-        <v>132</v>
+        <v>126</v>
       </c>
     </row>
     <row r="7" spans="1:7" ht="280.8" x14ac:dyDescent="0.3">
@@ -2116,10 +2116,10 @@
         <v>79</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>133</v>
+        <v>127</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>134</v>
+        <v>128</v>
       </c>
       <c r="D11" s="2" t="s">
         <v>8</v>
@@ -2128,7 +2128,7 @@
         <v>51</v>
       </c>
       <c r="F11" s="2" t="s">
-        <v>135</v>
+        <v>129</v>
       </c>
     </row>
     <row r="12" spans="1:7" ht="78" x14ac:dyDescent="0.3">
@@ -2136,10 +2136,10 @@
         <v>80</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>136</v>
+        <v>130</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>141</v>
+        <v>135</v>
       </c>
       <c r="D12" s="7" t="s">
         <v>67</v>
@@ -2148,10 +2148,10 @@
         <v>66</v>
       </c>
       <c r="F12" s="2" t="s">
-        <v>128</v>
+        <v>122</v>
       </c>
       <c r="G12" s="2" t="s">
-        <v>140</v>
+        <v>134</v>
       </c>
     </row>
     <row r="13" spans="1:7" ht="78" x14ac:dyDescent="0.3">
@@ -2159,10 +2159,10 @@
         <v>81</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>137</v>
+        <v>131</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>141</v>
+        <v>135</v>
       </c>
       <c r="D13" s="7" t="s">
         <v>67</v>
@@ -2171,10 +2171,10 @@
         <v>66</v>
       </c>
       <c r="F13" s="2" t="s">
-        <v>128</v>
+        <v>122</v>
       </c>
       <c r="G13" s="2" t="s">
-        <v>139</v>
+        <v>133</v>
       </c>
     </row>
     <row r="14" spans="1:7" ht="93.6" x14ac:dyDescent="0.3">
@@ -2194,10 +2194,10 @@
         <v>66</v>
       </c>
       <c r="F14" s="2" t="s">
-        <v>138</v>
+        <v>132</v>
       </c>
       <c r="G14" s="2" t="s">
-        <v>142</v>
+        <v>136</v>
       </c>
     </row>
     <row r="15" spans="1:7" ht="93.6" x14ac:dyDescent="0.3">
@@ -2205,10 +2205,10 @@
         <v>83</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>146</v>
+        <v>140</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>145</v>
+        <v>139</v>
       </c>
       <c r="D15" s="7" t="s">
         <v>67</v>
@@ -2217,10 +2217,10 @@
         <v>66</v>
       </c>
       <c r="F15" s="2" t="s">
-        <v>138</v>
+        <v>132</v>
       </c>
       <c r="G15" s="2" t="s">
-        <v>143</v>
+        <v>137</v>
       </c>
     </row>
     <row r="16" spans="1:7" ht="93.6" x14ac:dyDescent="0.3">
@@ -2228,10 +2228,10 @@
         <v>84</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>147</v>
+        <v>141</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>145</v>
+        <v>139</v>
       </c>
       <c r="D16" s="7" t="s">
         <v>67</v>
@@ -2240,10 +2240,10 @@
         <v>66</v>
       </c>
       <c r="F16" s="2" t="s">
+        <v>132</v>
+      </c>
+      <c r="G16" s="2" t="s">
         <v>138</v>
-      </c>
-      <c r="G16" s="2" t="s">
-        <v>144</v>
       </c>
     </row>
     <row r="17" spans="1:7" ht="78" x14ac:dyDescent="0.3">
@@ -2251,7 +2251,7 @@
         <v>85</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="C17" s="2" t="s">
         <v>108</v>
@@ -2274,7 +2274,7 @@
         <v>86</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>118</v>
+        <v>152</v>
       </c>
       <c r="C18" s="2" t="s">
         <v>108</v>
@@ -2297,7 +2297,7 @@
         <v>87</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>117</v>
+        <v>153</v>
       </c>
       <c r="C19" s="2" t="s">
         <v>108</v>
@@ -2320,7 +2320,7 @@
         <v>88</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>120</v>
+        <v>154</v>
       </c>
       <c r="C20" s="2" t="s">
         <v>108</v>
@@ -2343,7 +2343,7 @@
         <v>89</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>121</v>
+        <v>155</v>
       </c>
       <c r="C21" s="2" t="s">
         <v>108</v>
@@ -2366,7 +2366,7 @@
         <v>90</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>122</v>
+        <v>156</v>
       </c>
       <c r="C22" s="2" t="s">
         <v>108</v>
@@ -2389,7 +2389,7 @@
         <v>91</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>123</v>
+        <v>157</v>
       </c>
       <c r="C23" s="2" t="s">
         <v>108</v>
@@ -2412,7 +2412,7 @@
         <v>92</v>
       </c>
       <c r="B24" s="2" t="s">
-        <v>124</v>
+        <v>118</v>
       </c>
       <c r="C24" s="2" t="s">
         <v>108</v>
@@ -2435,7 +2435,7 @@
         <v>93</v>
       </c>
       <c r="B25" s="2" t="s">
-        <v>148</v>
+        <v>142</v>
       </c>
       <c r="C25" s="2" t="s">
         <v>65</v>
@@ -2447,7 +2447,7 @@
         <v>47</v>
       </c>
       <c r="F25" s="2" t="s">
-        <v>132</v>
+        <v>126</v>
       </c>
     </row>
     <row r="26" spans="1:7" ht="62.4" x14ac:dyDescent="0.3">
@@ -2455,7 +2455,7 @@
         <v>94</v>
       </c>
       <c r="B26" s="2" t="s">
-        <v>149</v>
+        <v>143</v>
       </c>
       <c r="C26" s="2" t="s">
         <v>65</v>
@@ -2467,7 +2467,7 @@
         <v>47</v>
       </c>
       <c r="F26" s="2" t="s">
-        <v>132</v>
+        <v>126</v>
       </c>
     </row>
     <row r="27" spans="1:7" ht="409.6" x14ac:dyDescent="0.3">
@@ -2475,10 +2475,10 @@
         <v>95</v>
       </c>
       <c r="B27" s="2" t="s">
-        <v>153</v>
+        <v>147</v>
       </c>
       <c r="C27" s="2" t="s">
-        <v>152</v>
+        <v>146</v>
       </c>
       <c r="D27" s="7" t="s">
         <v>67</v>
@@ -2487,10 +2487,10 @@
         <v>66</v>
       </c>
       <c r="F27" s="2" t="s">
-        <v>151</v>
+        <v>145</v>
       </c>
       <c r="G27" s="2" t="s">
-        <v>150</v>
+        <v>144</v>
       </c>
     </row>
     <row r="28" spans="1:7" ht="109.2" x14ac:dyDescent="0.3">
@@ -2498,10 +2498,10 @@
         <v>96</v>
       </c>
       <c r="B28" s="2" t="s">
-        <v>155</v>
+        <v>149</v>
       </c>
       <c r="C28" s="2" t="s">
-        <v>156</v>
+        <v>150</v>
       </c>
       <c r="D28" s="2" t="s">
         <v>36</v>
@@ -2510,10 +2510,10 @@
         <v>2019</v>
       </c>
       <c r="F28" s="2" t="s">
-        <v>157</v>
+        <v>151</v>
       </c>
       <c r="G28" s="2" t="s">
-        <v>154</v>
+        <v>148</v>
       </c>
     </row>
     <row r="29" spans="1:7" ht="109.2" x14ac:dyDescent="0.3">
@@ -2533,10 +2533,10 @@
         <v>2018</v>
       </c>
       <c r="F29" s="2" t="s">
-        <v>157</v>
+        <v>151</v>
       </c>
       <c r="G29" s="2" t="s">
-        <v>154</v>
+        <v>148</v>
       </c>
     </row>
     <row r="30" spans="1:7" ht="78" x14ac:dyDescent="0.3">
@@ -2544,10 +2544,10 @@
         <v>57</v>
       </c>
       <c r="B30" s="2" t="s">
-        <v>126</v>
+        <v>120</v>
       </c>
       <c r="C30" s="2" t="s">
-        <v>127</v>
+        <v>121</v>
       </c>
       <c r="D30" s="2" t="s">
         <v>67</v>
@@ -2556,10 +2556,10 @@
         <v>66</v>
       </c>
       <c r="F30" s="2" t="s">
-        <v>128</v>
+        <v>122</v>
       </c>
       <c r="G30" s="2" t="s">
-        <v>125</v>
+        <v>119</v>
       </c>
     </row>
   </sheetData>

</xml_diff>